<commit_message>
excel q and a
</commit_message>
<xml_diff>
--- a/data-sample/question_and_answer/q_and_a_sample.xlsx
+++ b/data-sample/question_and_answer/q_and_a_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\paul\projects\knowledgebase-elastic-rag\data-sample\question_and_answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27183D03-71E2-4903-87A8-4D20A6D8DF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A661A0-ED2C-4BCB-8B4A-000D069F35D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Question 1</t>
+    <t>How many people can I hire?</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
xl read and test
</commit_message>
<xml_diff>
--- a/data-sample/question_and_answer/q_and_a_sample.xlsx
+++ b/data-sample/question_and_answer/q_and_a_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\paul\projects\knowledgebase-elastic-rag\data-sample\question_and_answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A661A0-ED2C-4BCB-8B4A-000D069F35D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3C6CC-9EE0-461D-9136-858C45E34372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Question</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>How many people can I hire?</t>
+  </si>
+  <si>
+    <t>Is the grant available to a startup?</t>
   </si>
 </sst>
 </file>
@@ -354,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -385,6 +388,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit all changes pre merge
</commit_message>
<xml_diff>
--- a/data-sample/question_and_answer/q_and_a_sample.xlsx
+++ b/data-sample/question_and_answer/q_and_a_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\paul\projects\knowledgebase-elastic-rag\data-sample\question_and_answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3C6CC-9EE0-461D-9136-858C45E34372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119E356E-5DFD-41E8-834B-48D5F79FA630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>How many people can I hire?</t>
+    <t>Is the grant available to a startup?</t>
   </si>
   <si>
-    <t>Is the grant available to a startup?</t>
+    <t>I have a client who looking to hire a Chinese national with a recent masters in engineering. Is he eligible for support?</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +385,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -393,7 +393,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>